<commit_message>
Added and edited doc files
</commit_message>
<xml_diff>
--- a/doc/Netzplan.xlsx
+++ b/doc/Netzplan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\uib05241\AndroidStudioProjects\SolveMeDis\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03A096DA-E18F-4852-A55B-91AD1CBF0835}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D292389A-A8BB-4DCF-829B-36DC9BA0C639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>A</t>
   </si>
@@ -46,6 +46,21 @@
   </si>
   <si>
     <t>Client zu Server Kommunikation</t>
+  </si>
+  <si>
+    <t>Fertigstellen aller Features</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
   </si>
 </sst>
 </file>
@@ -69,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -225,11 +240,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -246,41 +283,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,15 +559,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>275064</xdr:colOff>
+      <xdr:colOff>278296</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>126380</xdr:rowOff>
+      <xdr:rowOff>133006</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>535258</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>130097</xdr:rowOff>
+      <xdr:rowOff>133007</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -532,9 +581,9 @@
         <xdr:cNvCxnSpPr/>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="3486615" y="3352800"/>
-          <a:ext cx="795453" cy="3717"/>
+        <a:xfrm>
+          <a:off x="3498574" y="3379789"/>
+          <a:ext cx="793675" cy="1"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -745,6 +794,209 @@
         <a:ln>
           <a:tailEnd type="triangle"/>
         </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>270164</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>529936</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>121227</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="13" name="Gerade Verbindung mit Pfeil 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D33B7B6-3EB6-4BD2-A28A-AA80E2A42C21}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6710721" y="1512705"/>
+          <a:ext cx="796485" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>263538</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>132522</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>263538</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>112643</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Gerader Verbinder 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDEBEC40-E623-48A1-A2A6-FC4B48CF2753}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9924373" y="1524000"/>
+          <a:ext cx="0" cy="1835426"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>529935</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>125896</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>265043</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>125896</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="17" name="Gerader Verbinder 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8BC8FF78-4DEE-4E91-9B0C-407F33B23DF3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9117344" y="1517374"/>
+          <a:ext cx="808534" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>265043</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="18" name="Gerader Verbinder 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0488FB8F-00A2-461B-AAF5-E1487E8869ED}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5900530" y="3362739"/>
+          <a:ext cx="4025348" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -1029,10 +1281,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B3:R17"/>
+  <dimension ref="B3:X17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.77734375" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1040,24 +1292,24 @@
     <col min="1" max="16384" width="7.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H3" s="14">
+    <row r="3" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H3" s="6">
         <v>5</v>
       </c>
-      <c r="L3" s="17">
+      <c r="L3" s="9">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="7"/>
+      <c r="K4" s="17"/>
     </row>
-    <row r="5" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I5" s="3">
         <v>3</v>
       </c>
@@ -1067,44 +1319,44 @@
       <c r="K5" s="5">
         <v>2</v>
       </c>
-      <c r="N5" s="14">
+      <c r="N5" s="6">
         <v>10</v>
       </c>
-      <c r="R5" s="17">
+      <c r="R5" s="9">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H6" s="15">
+    <row r="6" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="7">
         <v>7</v>
       </c>
-      <c r="L6" s="16">
+      <c r="L6" s="8">
         <v>10</v>
       </c>
-      <c r="O6" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="P6" s="8" t="s">
+      <c r="O6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="P6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="Q6" s="10"/>
+      <c r="Q6" s="13"/>
     </row>
-    <row r="7" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="O7" s="13"/>
-      <c r="P7" s="9"/>
-      <c r="Q7" s="11"/>
+    <row r="7" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O7" s="21"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="15"/>
     </row>
-    <row r="8" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14">
+    <row r="8" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="6">
         <v>0</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="9">
         <v>5</v>
       </c>
-      <c r="H8" s="14">
+      <c r="H8" s="6">
         <v>5</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="9">
         <v>10</v>
       </c>
       <c r="O8" s="3">
@@ -1117,29 +1369,35 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="17"/>
       <c r="I9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="N9" s="15">
+      <c r="K9" s="17"/>
+      <c r="N9" s="7">
         <v>10</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="8">
         <v>15</v>
       </c>
+      <c r="T9" s="6">
+        <v>15</v>
+      </c>
+      <c r="X9" s="9">
+        <v>20</v>
+      </c>
     </row>
-    <row r="10" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C10" s="3">
         <v>5</v>
       </c>
@@ -1158,63 +1416,100 @@
       <c r="K10" s="5">
         <v>0</v>
       </c>
+      <c r="U10" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="V10" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="W10" s="13"/>
     </row>
-    <row r="11" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="15">
+    <row r="11" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="7">
         <v>0</v>
       </c>
-      <c r="F11" s="16">
+      <c r="F11" s="8">
         <v>5</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="7">
         <v>5</v>
       </c>
-      <c r="L11" s="16">
+      <c r="L11" s="8">
         <v>10</v>
       </c>
+      <c r="U11" s="21"/>
+      <c r="V11" s="19"/>
+      <c r="W11" s="15"/>
     </row>
-    <row r="13" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H13" s="14">
+    <row r="12" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="U12" s="3">
         <v>5</v>
       </c>
-      <c r="L13" s="17">
+      <c r="V12" s="4">
+        <v>0</v>
+      </c>
+      <c r="W12" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H13" s="6">
+        <v>5</v>
+      </c>
+      <c r="L13" s="9">
         <v>8</v>
       </c>
+      <c r="T13" s="7">
+        <v>15</v>
+      </c>
+      <c r="X13" s="8">
+        <v>20</v>
+      </c>
     </row>
-    <row r="14" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I14" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8" t="s">
+    <row r="14" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="K14" s="10"/>
+      <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="2:18" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="I15" s="13"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="11"/>
+    <row r="15" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="11"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="15"/>
     </row>
-    <row r="16" spans="2:18" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:24" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I16" s="3">
         <v>3</v>
       </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="5"/>
+      <c r="J16" s="4">
+        <v>7</v>
+      </c>
+      <c r="K16" s="5">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" spans="8:12" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="H17" s="15"/>
-      <c r="L17" s="16"/>
+      <c r="H17" s="7">
+        <v>12</v>
+      </c>
+      <c r="L17" s="8">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="V10:W11"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:K15"/>
     <mergeCell ref="O6:O7"/>
     <mergeCell ref="P6:Q7"/>
     <mergeCell ref="D9:E9"/>
     <mergeCell ref="J4:K4"/>
     <mergeCell ref="J9:K9"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:K15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>